<commit_message>
Cleared up some Word HTML artefacts
</commit_message>
<xml_diff>
--- a/disasterinfosite/data/snuggets-es.xlsx
+++ b/disasterinfosite/data/snuggets-es.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="354">
   <si>
     <t>section</t>
   </si>
@@ -470,15 +470,6 @@
     <t>&lt;p&gt;Existe una &lt;b&gt;LIGERA PROBABILIDAD&lt;/b&gt; (5%) de que haya un terremoto de magnitud 7+ en la falla de Seattle en los próximos 50 años, pero si sucede, producirá daños. Los fuertes temblores dificultarán el caminar. &lt;b&gt;Los libros, la cristalería y otros elementos se caerán de los estantes. Algunas chimeneas y edificios de construcción deficiente sufrirán daños.&lt;/b&gt; &lt;a href="https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg" target="_blank"&gt;(mapa)&lt;/a&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Existe una &lt;b&gt;LIGERA PROBABILIDAD&lt;/b&gt; (5%) de que haya un terremoto de magnitud 7+ en la falla de Seattle en los próximos 50 años, pero si sucede, producirá daños. &lt;b&gt;Los temblores muy fuertes harán difícil mantenerse en pie. Los muebles se trasladarán y objetos caerán.&lt;/b&gt; Los daños serán importantes en edificios de mala construcción y moderados en edificios normales. &lt;a href="https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg" target="_blank"&gt;(mapa)&lt;/a&gt;&lt;br /&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target="_blank"&gt;&lt;img border=0 width=300 height=196 id="_x005F_x0000_i1057" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image004.jpg" alt="lick on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct"&gt;&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Existe una &lt;b&gt;LIGERA PROBABILIDAD&lt;/b&gt; (5%) de que haya un terremoto de magnitud 7+ en la falla de Seattle en los próximos 50 años, pero si sucede, producirá daños. &lt;b&gt;Los temblores muy fuertes harán difícil mantenerse en pie o conducir. Los muebles pesados caerán. Partes de edificios&lt;/b&gt; &lt;a href="http://www.seattle.gov/dpd/codesrules/changestocode/unreinforcedmasonrybuildings/whatwhy/" target="_blank"&gt;&lt;b&gt; URM&lt;/b&gt;&lt;/a&gt; &lt;b&gt; caerán y las casas con marcos de madera se trasladarán en los cimientos.&lt;/b&gt; &lt;a href="https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg" target="_blank"&gt;(mapa)&lt;/a&gt;&lt;br /&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target="_blank"&gt;&lt;img border=0 width=300 height=196 id="Picture 2" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image004.jpg" alt="lick on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct"&gt;&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Existe una &lt;b&gt;LIGERA PROBABILIDAD&lt;/b&gt; (5%) de que haya un terremoto de magnitud 7+ en la falla de Seattle en los próximos 50 años, pero si sucede, producirá daños. &lt;b&gt;Las sacudidas violentas provocarán pánico generalizado y aparecerán grietas en el piso. Se provocarán deslizamientos de tierra en pendientes pronunciadas y se producirá licuefacción en tierras saturadas.&lt;/b&gt; &lt;a href="https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg" target="_blank"&gt;(mapa)&lt;/a&gt;&lt;br /&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target="_blank"&gt;&lt;img border=0 width=300 height=196 id="Picture 3" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image004.jpg" alt="lick on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct"&gt;&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Usted se encuentra en una &lt;b&gt;zona de tsunami de ALTO RIESGO&lt;/b&gt;. Los niveles de agua superarán la altura de su cabeza entre unos pocos minutos hasta decenas de minutos después del terremoto. Una vez que se detengan los temblores, EVACUÉ INMEDIATAMENTE hacia terreno más elevado. &lt;a href="https://hazardready.org/seattle/static/img/data/Earthquake_Tsunami.jpg" target="_blank"&gt;(mapa)&lt;/a&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -845,9 +836,6 @@
     <t>Las fallas de represas son muy infrecuentes. Sin embargo, si la &lt;a href="https://goo.gl/maps/DpotpRjYDvG2" target="_blank"&gt;Represa Tolt River&lt;/a&gt; fallara, esta área se podría inundar &lt;a href="https://hazardready.org/seattle/static/img/data/Flood_DamInundation.jpg" target="_blank"&gt;(mapa)&lt;/a&gt; . Inscríbase para recibir alertas de inundaciones enviando un &lt;a href="https://green2.kingcounty.gov/floodalertsystem/" target="_blank"&gt;correo electrónico o mensaje de texto&lt;/a&gt;  o descargue la &lt;a href="http://kingcounty.gov/services/environment/water-and-land/flooding/warning-system/app.aspx" target="_blank"&gt;aplicación de alerta de inundación&lt;/a&gt; en su teléfono inteligente.</t>
   </si>
   <si>
-    <t>Se espera que las grandes tormentas aumenten en los próximos 50 años. Vendrán acompañadas de lluvia y nieve. Los ríos tendrán mayores caudales, lo que provocará mayores inundaciones en el otoño e invierno. Haga clic en la imagen para obtener más información.&lt;br /&gt;&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target="_blank"&gt;&lt;img border=0 width=140 height=125 id="Picture 11" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image014.png" alt="Climate Change Rivers Infographic"&gt;&lt;/a&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;ol&gt; &lt;li&gt;&lt;b&gt;PLANIFIQUE&lt;/b&gt;: haga un plan de qué hacer y dónde ir si el nivel del agua aumenta. &lt;b&gt;Tenga listos los artículos esenciales&lt;/b&gt; (certificados de nacimiento, documentos importantes, fotografías, etc.). Contrate un seguro contra inundaciones si lo necesita. &lt;/li&gt; &lt;li&gt;&lt;b&gt;PREPÁRESE:&lt;/b&gt; guarde los objetos valiosos y los productos químicos caseros por encima de los niveles de inundaciones y &lt;b&gt;aprenda a cortar los servicios públicos&lt;/b&gt; ( &lt;a href="http://www.seattle.gov/emergency-management/preparedness/prepare-your-home" target="_blank"&gt;agua, gas y electricidad&lt;/a&gt; ). &lt;/li&gt; &lt;/ol&gt;</t>
   </si>
   <si>
@@ -926,9 +914,6 @@
     <t>&lt;ol&gt; &lt;li&gt;&lt;b&gt;EVALÚE:&lt;/b&gt; si el área alrededor de su hogar pudiera estar propensa a deslizamientos de tierra &lt;b&gt;pida asesoría a expertos geotécnicos&lt;/b&gt;. Ellos pueden evaluar el peligro de deslizamientos de tierra o diseñar técnicas correctivas para reducir el riesgo de deslizamiento de tierra. &lt;/li&gt; &lt;li&gt;&lt;b&gt;REDUZCA EL RIESGO:&lt;/b&gt; plante capas vegetales en pendientes o construya un muro de retención para &lt;b&gt;estabilizar laderas.&lt;/b&gt; &lt;/li&gt; &lt;li&gt;&lt;b&gt;PREPÁRESE:&lt;/b&gt; &lt;b&gt;haga un kit de suministros y un plan familiar&lt;/b&gt; designando al menos dos rutas de evacuación. &lt;/li&gt; &lt;/ol&gt;</t>
   </si>
   <si>
-    <t>&lt;b&gt;Su mejor protección es mantenerse fuera del recorrido de un deslizamiento de tierra o un flujo de escombros.&lt;/b&gt; El Estudio Geológico de EE.&amp;nbsp;UU. también recomendó lo siguiente: &lt;ul&gt; &lt;li&gt;&lt;b&gt;MANTÉNGASE ALERTA: preste atención a sonidos inusuales.&lt;/b&gt; Las lluvias intensas y cortas pueden ser particularmente peligrosas, especialmente después de largos períodos de lluvias torrenciales y clima húmedo. &lt;/li&gt; &lt;li&gt;&lt;b&gt;CONSIDERE IRSE:&lt;/b&gt; si está en un área propensa a deslizamientos de tierra y flujos de escombros, considere irse, si es seguro hacerlo. Si decide quedarse en casa, vaya a un segundo piso, si es posible. &lt;/li&gt; &lt;li&gt;&lt;b&gt;PRESTE ATENCIÓN A LOS NIVELES DE ARROYOS:&lt;/b&gt; si está cerca de un arroyo o canal, &lt;b&gt;esté atento a cualquier aumento o disminución de la corriente y todo cambio de agua clara a lodosa.&lt;/b&gt; Esto podría ser un indicador de actividad de deslizamiento de tierras aguas arriba. ¡NO SE DEMORE! Sálvese usted, no sus pertenencias. &lt;/li&gt; &lt;/ul&gt;Puede encontrar más consejos sobre deslizamientos de tierra en USGS &lt;a href="http://landslides.usgs.gov/learn/prepare.php" target="_blank"&gt;aquí&lt;/a&gt; . &lt;img border=0 width=387 height=97 id="Picture 34" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image020.png" alt="This is a panel of three cartoon images showing what to do during a landslide if indoors, near slide, or in slide"&gt;</t>
-  </si>
-  <si>
     <t>&lt;b&gt;ESTÉ PREPARADO PARA LAS INUNDACIONES (los deslizamientos de tierra con frecuencia bloquean los ríos y pueden provocar que los ríos retrocedan e inunden).&lt;/b&gt;&lt;ul&gt; &lt;li&gt; Manténgase lejos del deslizamiento. Pueden ocurrir otros deslizamientos después del deslizamiento principal. &lt;/li&gt; &lt;li&gt; Una vez que esté seguro, revise si hay personas heridas o atrapadas. &lt;/li&gt; &lt;li&gt; Revise si hay líneas de servicios públicos dañadas e informe todo daño a su empresa de servicios públicos. &lt;/li&gt; &lt;li&gt; Escuche los medios locales o la radio meteorológica de la NOAA para acceder a información actualizada. &lt;/li&gt; &lt;/ul&gt;</t>
   </si>
   <si>
@@ -980,21 +965,12 @@
     <t>&lt;p&gt;&lt;b&gt;Es improbable, pero si vive cerca de una zona forestal, puede sufrir un incendio forestal.&lt;/b&gt; El HUMO de incendios forestales distantes puede recorrer grandes distancias y puede ser un factor, incluso si nada se está quemando en el área. Consulte su calidad del aire local &lt;a href="http://www.pscleanair.org/airquality/ourairquality/Pages/default.aspx" target="_blank"&gt;aquí&lt;/a&gt;.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;La cantidad de &lt;b&gt;incendios forestales en el noroeste del Pacífico ya aumentó significativamente en las últimas décadas.&lt;/b&gt; Esta tendencia es probable que continúe con veranos más secos y con más tormentas (piense en los rayos que inician incendios). Grandes áreas de bosques pueden quemarse y enviar humo a la atmósfera. Haga clic en la imagen para obtener más información.&lt;BR /&gt;&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target="_blank"&gt;&lt;img border=0 width=144 height=144 id="Picture 26" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image024.png" alt="limate Change Forest Infographic"&gt;&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;¿Huele o ve humo? ¿Ha sido una temporada de clima seco? Podría ser un incendio forestal. Aléjese de incendios activos y, si ve que se inicia uno, llame al 9-1-1 para informarlo.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;HAGA LUGAR&lt;/b&gt;: proteja las vidas y los bienes creando un &lt;b&gt;espacio adaptado para los incendios alrededor de su casa&lt;/b&gt;, cobertizo y negocio. Para descubrir cómo hacerlo, ingrese a &lt;a href="http://www.firewise.org/wildfire-preparedness.aspx" target="_blank"&gt;firewise.org&lt;/a&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;OBSERVE EL CLIMA:&lt;/b&gt; unos pocos días soleados pueden secar los bosques lo suficiente para que se incendien. Las condiciones ventosas pueden provocar que los incendios forestales se salgan de control rápidamente. &lt;img border=0 width=301 height=264 id="_x005F_x0000_i1034" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image025.png" alt="his is an image of ways to prevent wildfire around your home. They include screening decks, pruning trees 6-10 feet from the ground, using fire-resistant wall and roof materials, keeping plants watered, and making sure your driveway can accommodate an emergency vehicle"&gt;&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t>&lt;ul&gt;&lt;li&gt; Regrese a su casa una vez que las autoridades digan que es seguro hacerlo.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Tenga cuidado al ingresar a áreas quemadas&lt;/b&gt; ya que aún podría haber peligros.&lt;/li&gt;&lt;li&gt; Revise exhaustivamente para determinar si hay humo o brasas ocultas.&lt;/li&gt;&lt;li&gt;&lt;b&gt;Saque fotografías de los daños&lt;/b&gt; para la aseguradora.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;MANTÉNGASE INFORMADO:&lt;/b&gt; escuche las alertas de emergencias locales en la radio o la televisión y esté listo para evacuar si fuera necesario. &lt;/li&gt; &lt;li&gt;&lt;b&gt;ELIMINE LOS ELEMENTOS INFLAMABLES:&lt;/b&gt; quite los materiales de su propiedad y alrededor de esta que pudieran prenderse fuego (sillas de patio, mesas, etcétera). &lt;/li&gt; &lt;li&gt;&lt;b&gt;PREPARE SU CASA:&lt;/b&gt; - traslade los muebles tapizados lejos de las ventanas. Cierre puertas y ventanas, no las trabe. &lt;/li&gt; &lt;/ul&gt; &lt;img border=0 width=419 height=89 id="Picture 37" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image026.png"&gt;</t>
-  </si>
-  <si>
     <t>&lt;/p&gt;Si cree que su propiedad puede estar en riesgo, &lt;b&gt;el Condado King tiene información para propietarios, programas de incentivo y talleres de capacitación de anfitriones.&lt;/b&gt; Puede obtener más información &lt;a href="http://www.kingcounty.gov/environment/water-and-land/forestry.aspx" target="_blank"&gt;aquí&lt;/a&gt;.&lt;/p&gt;</t>
   </si>
   <si>
@@ -1025,9 +1001,6 @@
     <t>&lt;p&gt;Durante una erupción, escuche las noticias para ver actualizaciones de emergencia y siga las instrucciones de emergencia.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;b&gt;EN UNA ZONA DE LAHARES: acuda a tierras más altas inmediatamente.&lt;/b&gt;&lt;/li&gt; &lt;li&gt;&lt;b&gt;AFUERA:&lt;/b&gt; cúbrase boca, nariz y cuerpo para evitar la irritación. &lt;b&gt;Busque refugio.&lt;/b&gt; &lt;/li&gt; &lt;li&gt;&lt;b&gt;ADENTRO: mantenga las puertas y la ventilación de su casa cerradas y quédese adentro, a menos que se le indique lo contrario.&lt;/b&gt; Coloque toallas húmedas debajo de las puertas y tape con cinta las ventanas con corrientes de aire. Mantenga apagados los motores de automóviles y camiones para evitar daños por taponamiento por cenizas. Proteja animales y maquinarias haciéndolos ingresar o manteniéndolos en un área cubierta.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Una vez que haya desaparecido el riesgo inmediato por una erupción, la acción más importante será limpiar las cenizas. &lt;img border=0 width=337 height=129 id="Picture 43" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image030.png" alt="This image shows two graders shoveling inches of ashfall from Saint Helens' eruption"&gt;&lt;/p&gt; &lt;ul&gt; &lt;li&gt; Utilice gafas protectoras y una máscara facial al aire libre. &lt;b&gt;La calidad del aire será mala.&lt;/b&gt; &lt;/li&gt; &lt;li&gt;&lt;b&gt;Evite hacer andar motores de vehículos.&lt;/b&gt; Si debe manejar, hágalo despacio (a menos de 35 MPH) y controle el aceite, los filtros de aceite y los filtros de aire frecuentemente. &lt;/li&gt; &lt;li&gt; La lluvia de cenizas es muy pesada y puede hacer que los edificios colapsen. Si es seguro hacerlo, &lt;b&gt;quite la ceniza de techos y canalones de lluvia&lt;/b&gt;. &lt;/li&gt; &lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Puede obtener más información acerca del Monte Rainier y los posibles peligros en diferentes fuentes:&lt;/p&gt; &lt;ul&gt; &lt;li&gt; &lt;a href="https://volcanoes.usgs.gov/volcanoes/mount_rainier/" target="_blank"&gt;Monitoreo y otra información&lt;/a&gt; - Estudio Geológico de EE.&amp;nbsp;UU. &lt;/li&gt; &lt;li&gt; &lt;a href="http://www.kingcounty.gov/depts/emergency-management/hazards/volcano.aspx" target=blank&gt; Información general del Condado King&lt;/a&gt; &amp;nbsp;- Condado King &lt;/li&gt; &lt;li&gt; &lt;a href="https://www.nps.gov/mora/planyourvisit/geohazards.htm" target="_blank"&gt;Peligros geológicos en Rainier&lt;/a&gt;  - Servicio de Parques Nacionales &lt;/li&gt; &lt;li&gt; &lt;a href="http://www.pnsn.org/volcanoes/mount-rainier" target="_blank"&gt;Terremotos cerca de Rainier&lt;/a&gt; - Red Sísmica del Noroeste del Pacífico &lt;/li&gt; &lt;/ul&gt;</t>
   </si>
   <si>
@@ -1040,9 +1013,6 @@
     <t>&lt;p&gt;Un evento de nevadas copiosas puede provocar problemas importantes en los transportes, los servicios de seguridad pública y los servicios públicos. &lt;b&gt;La energía se puede cortar durante muchos días.&lt;/b&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;b&gt;El noroeste del Pacífico se verá afectado por tormentas más fuertes en los próximos 50 años.&lt;/b&gt; Pueden provocar fuertes vientos y lluvias torrenciales que provoquen inundaciones. Las actividades invernales se verán afectadas. 2015 tuvo los niveles de nieve acumulada más bajos que se hayan registrado con solo el 4% del promedio. Los inviernos cálidos establecerán las condiciones para sequías en todo el estado. Haga clic en la imagen para obtener más información.&lt;br&gt; &lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target="_blank"&gt;&lt;img border=0 width=144 height=144 id="Picture 32" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image031.png" alt="limate Change Winter Infographic"&gt;&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Los meteorólogos se han esforzado mucho por pronosticar las tormentas de nieve y hielo. &lt;b&gt;Preste atención a los pronósticos locales del tiempo e inscríbase en los sistemas de alerta de advertencia disponibles&lt;/b&gt; ( &lt;a href="http://alert.seattle.gov/" target="_blank"&gt;Alertas Seattle&lt;/a&gt; y &lt;a href="http://www.kingcounty.gov/depts/emergency-management/alert-king-county.aspx" target="_blank"&gt;Alertas Condado King&lt;/a&gt;) para asegurarse de obtener información actualizada acerca de futuro mal clima.&lt;/p&gt;</t>
   </si>
   <si>
@@ -1067,18 +1037,12 @@
     <t>&lt;p&gt;El calor intenso puede durar días causando que en las comunidades haya un incremento de enfermedades relacionadas con el calor, esto incluye los GOLPES DE CALOR y las INSOLACIONES. Las altas temperaturas, las condiciones secas y la mayor probabilidad de rayos pueden provocar incendios forestales.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Julio de 2015 fue el mes más caluroso de la historia. &lt;b&gt;La temperatura anual promedio se proyecta con un incremento de entre 3 y 10 grados Fahrenheit para 2100.&lt;/b&gt; Los residentes de Washington tendrán menos lluvias en verano, pero la lluvia que haya será más intensa (piense en aguaceros). Haga clic en la imagen para obtener más información.&lt;br&gt; &lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target="_blank"&gt;&lt;img border=0 width=153 height=131 id="Picture 38" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image033.png" alt="limate Change Storm Infographic"&gt;&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Los golpes de calor y las insolaciones son enfermedades graves que pueden aparecer cuando una persona se expone al calor extremo.&lt;/p&gt;&lt;div style="display: inline-block; width: 35%; vertical-align: top;"&gt;&lt;b&gt;SÍNTOMAS DE GOLPE DE CALOR:&lt;/b&gt;&lt;/p&gt; &lt;ul style='margin-top:0in' type=disc&gt; &lt;li&gt; Mucha sudoración &lt;/li&gt; &lt;li&gt; Debilidad &lt;/li&gt; &lt;li&gt; Pulso débil &lt;/li&gt; &lt;li&gt; Desmayos &lt;/li&gt; &lt;li&gt; Vómitos &lt;/li&gt; &lt;li&gt; Piel fría y pálida &lt;/li&gt; &lt;/ul&gt;&lt;/div&gt;&lt;div style="display: inline-block; width: 35%; vertical-align: top;"&gt;&lt;b&gt;SÍNTOMAS DE INSOLACIÓN:&lt;/b&gt;&lt;/p&gt; &lt;ul style='margin-top:0in' type=disc&gt; &lt;li&gt; Alta temperatura corporal (103&amp;nbsp;°F o más) &lt;/li&gt; &lt;li&gt; Piel caliente y seca &lt;/li&gt; &lt;li&gt; Pulso acelerado y fuerte &lt;/li&gt; &lt;li&gt; Posible pérdida de la conciencia &lt;/li&gt; &lt;/ul&gt;&lt;/div&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Los adultos mayores, los niños pequeños y las personas con enfermedades mentales y crónicas tienen mayor riesgo de problemas cardíacos.&lt;/p&gt; &lt;ol&gt; &lt;li&gt;&lt;b&gt;SEPA LOS SÍNTOMAS:&lt;/b&gt; las enfermedades relacionadas con el calor pueden aparecer rápidamente. Sepa cuál de sus vecinos puede estar en riesgo. &lt;/li&gt; &lt;li&gt;&lt;b&gt;MANTÉNGASE INFORMADO:&lt;/b&gt; escuche las noticias locales para obtener información general y las direcciones de los &lt;b&gt;centros de refrigeración&lt;/b&gt; (espacios públicos que pueden utilizar los residentes para mantenerse frescos). &lt;/li&gt; &lt;/ol&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt; &lt;li&gt;&lt;b&gt;MANTÉNGASE FRESCO:&lt;/b&gt; quédese adentro y, si es posible, en un lugar con aire acondicionado (centro comercial, biblioteca, teatro, etc.). Limite las actividades al aire libre. &lt;/li&gt; &lt;li&gt;&lt;b&gt;PROTEJA LA PIEL:&lt;/b&gt; utilice prendas livianas, holgadas y con colores claros. Un sombrero de ala ancha, lentes de sol y pantalla solar serán de ayuda. &lt;/li&gt; &lt;li&gt;&lt;b&gt;AGUA POTABLE:&lt;/b&gt; tome mucho líquido (evite la cafeína, el alcohol y las bebidas azucaradas) y lleve consigo una botella de agua. &lt;/li&gt; &lt;li&gt;&lt;b&gt;PIENSE EN LOS DEMÁS:&lt;/b&gt; mantenga a los niños y las mascotas fuera de automóviles calientes. Controle con frecuencia a familias, amigos y vecinos en riesgo. &lt;/li&gt; &lt;/ul&gt; &lt;p&gt;&lt;img border=0 width=355 height=87 id="Picture 41" src="Snugget_for_translation_Edits_Carson_5_15_17_SPL.fld/image034.png" alt="his is a panel of three images of what to do during bad summer weather. Stay Cool, Protect Skin, and Drink Water."&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;ul&gt; &lt;li&gt; Utilice cortinas para &lt;b&gt;cubrir las ventanas y mantener el aire fresco en el interior.&lt;/b&gt; &lt;/li&gt; &lt;li&gt;&lt;b&gt;Piense en comprar un sistema de aire acondicionado&lt;/b&gt; o instalar burletes en los lugares por donde se cuela el aire caliente. &lt;/li&gt; &lt;li&gt;&lt;b&gt;OPCIÓN DE BAJO PRESUPUESTO:&lt;/b&gt; construya reflectores de calor (para utilizar entre ventanas y cortinas), como cartón cubierto de papel de aluminio, para reflejar el calor hacia el exterior. Haga clic &lt;a href="http://www.instructables.com/id/Heat-blocking-curtains/" target="_blank"&gt;aquí&lt;/a&gt; para instrucciones sobre cómo hacerlo usted mismo. &lt;/li&gt; &lt;/ul&gt;</t>
   </si>
   <si>
@@ -1086,6 +1050,45 @@
   </si>
   <si>
     <t>&lt;p&gt;En 2015, el Condado King tuvo una cantidad récord de días que superaron los 90°F. &lt;b&gt;Julio de 2015 fue el mes más caluroso de la historia en el Condado King.&lt;/b&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>¿Ha estado lloviendo intensamente o durante muchos días? ¿El aumento de la temperatura causó un rápido deshielo en las montañas? ¿Parecen altos los niveles del agua en los ríos locales? Las posibilidades de inundación podrían estar en aumento. Consulte los informes de noticias del servicio meteorológico para ver si hay alertas locales.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Su mejor protección es mantenerse fuera del recorrido de un deslizamiento de tierra o un flujo de escombros.&lt;/b&gt; El Estudio Geológico de EE.&amp;nbsp;UU. también recomendó lo siguiente: &lt;ul&gt; &lt;li&gt;&lt;b&gt;MANTÉNGASE ALERTA: preste atención a sonidos inusuales.&lt;/b&gt; Las lluvias intensas y cortas pueden ser particularmente peligrosas, especialmente después de largos períodos de lluvias torrenciales y clima húmedo. &lt;/li&gt; &lt;li&gt;&lt;b&gt;CONSIDERE IRSE:&lt;/b&gt; si está en un área propensa a deslizamientos de tierra y flujos de escombros, considere irse, si es seguro hacerlo. Si decide quedarse en casa, vaya a un segundo piso, si es posible. &lt;/li&gt; &lt;li&gt;&lt;b&gt;PRESTE ATENCIÓN A LOS NIVELES DE ARROYOS:&lt;/b&gt; si está cerca de un arroyo o canal, &lt;b&gt;esté atento a cualquier aumento o disminución de la corriente y todo cambio de agua clara a lodosa.&lt;/b&gt; Esto podría ser un indicador de actividad de deslizamiento de tierras aguas arriba. ¡NO SE DEMORE! Sálvese usted, no sus pertenencias. &lt;/li&gt; &lt;/ul&gt;Puede encontrar más consejos sobre deslizamientos de tierra en USGS &lt;a href="http://landslides.usgs.gov/learn/prepare.php" target="_blank"&gt;aquí&lt;/a&gt; . &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Landslide_during.jpg" alt="This is a panel of three cartoon images showing what to do during a landslide if indoors, near slide, or in slide"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Existe una &lt;b&gt;LIGERA PROBABILIDAD&lt;/b&gt; (5%) de que haya un terremoto de magnitud 7+ en la falla de Seattle en los próximos 50 años, pero si sucede, producirá daños. &lt;b&gt;Los temblores muy fuertes harán difícil mantenerse en pie. Los muebles se trasladarán y objetos caerán.&lt;/b&gt; Los daños serán importantes en edificios de mala construcción y moderados en edificios normales. &lt;a href="https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg" target="_blank"&gt;(mapa)&lt;/a&gt;&lt;br /&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target="_blank"&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="Click on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Existe una &lt;b&gt;LIGERA PROBABILIDAD&lt;/b&gt; (5%) de que haya un terremoto de magnitud 7+ en la falla de Seattle en los próximos 50 años, pero si sucede, producirá daños. &lt;b&gt;Los temblores muy fuertes harán difícil mantenerse en pie o conducir. Los muebles pesados caerán. Partes de edificios&lt;/b&gt; &lt;a href="http://www.seattle.gov/dpd/codesrules/changestocode/unreinforcedmasonrybuildings/whatwhy/" target="_blank"&gt;&lt;b&gt; URM&lt;/b&gt;&lt;/a&gt; &lt;b&gt; caerán y las casas con marcos de madera se trasladarán en los cimientos.&lt;/b&gt; &lt;a href="https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg" target="_blank"&gt;(mapa)&lt;/a&gt;&lt;br /&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target="_blank"&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="lick on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Existe una &lt;b&gt;LIGERA PROBABILIDAD&lt;/b&gt; (5%) de que haya un terremoto de magnitud 7+ en la falla de Seattle en los próximos 50 años, pero si sucede, producirá daños. &lt;b&gt;Las sacudidas violentas provocarán pánico generalizado y aparecerán grietas en el piso. Se provocarán deslizamientos de tierra en pendientes pronunciadas y se producirá licuefacción en tierras saturadas.&lt;/b&gt; &lt;a href="https://hazardready.org/seattle/static/img/data/Earthquake_Seattle.jpg" target="_blank"&gt;(mapa)&lt;/a&gt;&lt;br /&gt;&lt;a href="https://www.youtube.com/watch?v=hos_uIKwC-c" target="_blank"&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/WSDOT_sim.jpg" alt="lick on this image to be taken to a video of a simulated magnitude 7 earthquake and the impacts along the Alaskan Way Viaduct"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Se espera que las grandes tormentas aumenten en los próximos 50 años. Vendrán acompañadas de lluvia y nieve. Los ríos tendrán mayores caudales, lo que provocará mayores inundaciones en el otoño e invierno. Haga clic en la imagen para obtener más información.&lt;br /&gt;&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target="_blank"&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Rivers.jpg" alt="Climate Change Rivers Infographic"&gt;&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;La cantidad de &lt;b&gt;incendios forestales en el noroeste del Pacífico ya aumentó significativamente en las últimas décadas.&lt;/b&gt; Esta tendencia es probable que continúe con veranos más secos y con más tormentas (piense en los rayos que inician incendios). Grandes áreas de bosques pueden quemarse y enviar humo a la atmósfera. Haga clic en la imagen para obtener más información.&lt;BR /&gt;&lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target="_blank"&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Forests.jpg" alt="Climate Change Forest Infographic"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;b&gt;HAGA LUGAR&lt;/b&gt;: proteja las vidas y los bienes creando un &lt;b&gt;espacio adaptado para los incendios alrededor de su casa&lt;/b&gt;, cobertizo y negocio. Para descubrir cómo hacerlo, ingrese a &lt;a href="http://www.firewise.org/wildfire-preparedness.aspx" target="_blank"&gt;firewise.org&lt;/a&gt;.&lt;/li&gt;&lt;li&gt;&lt;b&gt;OBSERVE EL CLIMA:&lt;/b&gt; unos pocos días soleados pueden secar los bosques lo suficiente para que se incendien. Las condiciones ventosas pueden provocar que los incendios forestales se salgan de control rápidamente. &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Firewise_Brochure.jpg" alt="his is an image of ways to prevent wildfire around your home. They include screening decks, pruning trees 6-10 feet from the ground, using fire-resistant wall and roof materials, keeping plants watered, and making sure your driveway can accommodate an emergency vehicle"&gt;&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;b&gt;MANTÉNGASE INFORMADO:&lt;/b&gt; escuche las alertas de emergencias locales en la radio o la televisión y esté listo para evacuar si fuera necesario. &lt;/li&gt; &lt;li&gt;&lt;b&gt;ELIMINE LOS ELEMENTOS INFLAMABLES:&lt;/b&gt; quite los materiales de su propiedad y alrededor de esta que pudieran prenderse fuego (sillas de patio, mesas, etcétera). &lt;/li&gt; &lt;li&gt;&lt;b&gt;PREPARE SU CASA:&lt;/b&gt; - traslade los muebles tapizados lejos de las ventanas. Cierre puertas y ventanas, no las trabe. &lt;/li&gt; &lt;/ul&gt; &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Fire_during.jpg"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Una vez que haya desaparecido el riesgo inmediato por una erupción, la acción más importante será limpiar las cenizas. &lt;img src="https://hazardready.org/images/seattle-ready/snuggets/MtStHel_Yakima_graders.jpg" alt="This image shows two graders shoveling inches of ashfall from Saint Helens' eruption"&gt;&lt;/p&gt; &lt;ul&gt; &lt;li&gt; Utilice gafas protectoras y una máscara facial al aire libre. &lt;b&gt;La calidad del aire será mala.&lt;/b&gt; &lt;/li&gt; &lt;li&gt;&lt;b&gt;Evite hacer andar motores de vehículos.&lt;/b&gt; Si debe manejar, hágalo despacio (a menos de 35 MPH) y controle el aceite, los filtros de aceite y los filtros de aire frecuentemente. &lt;/li&gt; &lt;li&gt; La lluvia de cenizas es muy pesada y puede hacer que los edificios colapsen. Si es seguro hacerlo, &lt;b&gt;quite la ceniza de techos y canalones de lluvia&lt;/b&gt;. &lt;/li&gt; &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;El noroeste del Pacífico se verá afectado por tormentas más fuertes en los próximos 50 años.&lt;/b&gt; Pueden provocar fuertes vientos y lluvias torrenciales que provoquen inundaciones. Las actividades invernales se verán afectadas. 2015 tuvo los niveles de nieve acumulada más bajos que se hayan registrado con solo el 4% del promedio. Los inviernos cálidos establecerán las condiciones para sequías en todo el estado. Haga clic en la imagen para obtener más información.&lt;br&gt; &lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target="_blank"&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Winter.jpg" alt="Climate Change Winter Infographic"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Julio de 2015 fue el mes más caluroso de la historia. &lt;b&gt;La temperatura anual promedio se proyecta con un incremento de entre 3 y 10 grados Fahrenheit para 2100.&lt;/b&gt; Los residentes de Washington tendrán menos lluvias en verano, pero la lluvia que haya será más intensa (piense en aguaceros). Haga clic en la imagen para obtener más información.&lt;br&gt; &lt;a href="http://kingcounty.gov/services/environment/climate/why-act/infographic.aspx" target="_blank"&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Climate_Storms.jpg" alt="limate Change Storm Infographic"&gt;&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt; &lt;li&gt;&lt;b&gt;MANTÉNGASE FRESCO:&lt;/b&gt; quédese adentro y, si es posible, en un lugar con aire acondicionado (centro comercial, biblioteca, teatro, etc.). Limite las actividades al aire libre. &lt;/li&gt; &lt;li&gt;&lt;b&gt;PROTEJA LA PIEL:&lt;/b&gt; utilice prendas livianas, holgadas y con colores claros. Un sombrero de ala ancha, lentes de sol y pantalla solar serán de ayuda. &lt;/li&gt; &lt;li&gt;&lt;b&gt;AGUA POTABLE:&lt;/b&gt; tome mucho líquido (evite la cafeína, el alcohol y las bebidas azucaradas) y lleve consigo una botella de agua. &lt;/li&gt; &lt;li&gt;&lt;b&gt;PIENSE EN LOS DEMÁS:&lt;/b&gt; mantenga a los niños y las mascotas fuera de automóviles calientes. Controle con frecuencia a familias, amigos y vecinos en riesgo. &lt;/li&gt; &lt;/ul&gt; &lt;p&gt;&lt;img src="https://hazardready.org/images/seattle-ready/snuggets/Summer_during.jpg" alt="his is a panel of three images of what to do during bad summer weather. Stay Cool, Protect Skin, and Drink Water."&gt;&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -2936,10 +2939,10 @@
   <dimension ref="A1:H292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D254" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H293" sqref="H293"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3130,7 +3133,7 @@
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5" t="s">
-        <v>147</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3154,7 +3157,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5" t="s">
-        <v>148</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3178,7 +3181,7 @@
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
-        <v>149</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3294,7 +3297,7 @@
         <v>18</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -3318,7 +3321,7 @@
         <v>18</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -3342,7 +3345,7 @@
         <v>18</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -3366,7 +3369,7 @@
         <v>19</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -3390,7 +3393,7 @@
         <v>18</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -3414,7 +3417,7 @@
         <v>20</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -3448,7 +3451,7 @@
         <v>24</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -3472,7 +3475,7 @@
         <v>26</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -3496,7 +3499,7 @@
         <v>28</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -3520,7 +3523,7 @@
         <v>30</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -3544,7 +3547,7 @@
         <v>32</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -3568,7 +3571,7 @@
         <v>34</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -3592,7 +3595,7 @@
         <v>36</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -3616,7 +3619,7 @@
         <v>38</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3640,7 +3643,7 @@
         <v>40</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -3674,7 +3677,7 @@
         <v>43</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -3698,7 +3701,7 @@
         <v>43</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -3722,7 +3725,7 @@
         <v>43</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -3746,7 +3749,7 @@
         <v>43</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -3770,7 +3773,7 @@
         <v>43</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -3804,7 +3807,7 @@
         <v>47</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -3836,7 +3839,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -3858,7 +3861,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -3880,7 +3883,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -3912,7 +3915,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -3934,7 +3937,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -3956,7 +3959,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -3978,7 +3981,7 @@
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -4000,7 +4003,7 @@
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -4022,7 +4025,7 @@
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -4044,7 +4047,7 @@
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -4066,7 +4069,7 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -4088,7 +4091,7 @@
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
@@ -4110,7 +4113,7 @@
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -4132,7 +4135,7 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -4154,7 +4157,7 @@
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -4176,7 +4179,7 @@
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -4198,7 +4201,7 @@
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -4220,7 +4223,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -4242,7 +4245,7 @@
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -4264,7 +4267,7 @@
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -4286,7 +4289,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -4308,7 +4311,7 @@
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -4330,7 +4333,7 @@
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -4352,7 +4355,7 @@
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="H65" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -4374,7 +4377,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="H66" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -4396,7 +4399,7 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -4418,7 +4421,7 @@
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -4440,7 +4443,7 @@
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -4462,7 +4465,7 @@
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -4484,7 +4487,7 @@
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -4506,7 +4509,7 @@
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="H72" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -4528,7 +4531,7 @@
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -4550,7 +4553,7 @@
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="H74" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -4572,7 +4575,7 @@
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
       <c r="H75" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -4594,7 +4597,7 @@
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -4616,7 +4619,7 @@
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -4638,7 +4641,7 @@
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
       <c r="H78" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -4660,7 +4663,7 @@
       <c r="F79" s="5"/>
       <c r="G79" s="5"/>
       <c r="H79" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -4682,7 +4685,7 @@
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
       <c r="H80" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -4704,7 +4707,7 @@
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -4726,7 +4729,7 @@
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
       <c r="H82" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -4748,7 +4751,7 @@
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -4770,7 +4773,7 @@
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -4792,7 +4795,7 @@
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -4814,7 +4817,7 @@
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -4836,7 +4839,7 @@
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -4858,7 +4861,7 @@
       <c r="F88" s="5"/>
       <c r="G88" s="5"/>
       <c r="H88" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -4880,7 +4883,7 @@
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
       <c r="H89" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -4902,7 +4905,7 @@
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -4924,7 +4927,7 @@
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -4946,7 +4949,7 @@
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -4968,7 +4971,7 @@
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
       <c r="H93" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -4990,7 +4993,7 @@
       <c r="F94" s="5"/>
       <c r="G94" s="5"/>
       <c r="H94" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -5012,7 +5015,7 @@
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
       <c r="H95" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -5034,7 +5037,7 @@
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
       <c r="H96" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -5056,7 +5059,7 @@
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
       <c r="H97" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -5078,7 +5081,7 @@
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
       <c r="H98" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -5100,7 +5103,7 @@
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
       <c r="H99" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -5122,7 +5125,7 @@
       <c r="F100" s="5"/>
       <c r="G100" s="5"/>
       <c r="H100" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -5144,7 +5147,7 @@
       <c r="F101" s="5"/>
       <c r="G101" s="5"/>
       <c r="H101" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -5166,7 +5169,7 @@
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
       <c r="H102" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -5188,7 +5191,7 @@
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
       <c r="H103" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -5210,7 +5213,7 @@
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
       <c r="H104" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -5232,7 +5235,7 @@
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
       <c r="H105" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -5254,7 +5257,7 @@
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
       <c r="H106" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -5276,7 +5279,7 @@
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
       <c r="H107" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -5298,7 +5301,7 @@
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
       <c r="H108" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -5320,7 +5323,7 @@
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
       <c r="H109" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -5352,7 +5355,7 @@
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
       <c r="H111" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -5396,7 +5399,7 @@
       </c>
       <c r="G114" s="5"/>
       <c r="H114" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -5420,7 +5423,7 @@
       </c>
       <c r="G115" s="5"/>
       <c r="H115" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -5444,7 +5447,7 @@
       </c>
       <c r="G116" s="5"/>
       <c r="H116" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -5468,7 +5471,7 @@
       </c>
       <c r="G117" s="5"/>
       <c r="H117" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -5492,7 +5495,7 @@
       </c>
       <c r="G118" s="5"/>
       <c r="H118" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -5516,7 +5519,7 @@
       </c>
       <c r="G119" s="5"/>
       <c r="H119" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -5540,7 +5543,7 @@
       </c>
       <c r="G120" s="5"/>
       <c r="H120" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -5564,7 +5567,7 @@
       </c>
       <c r="G121" s="5"/>
       <c r="H121" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -5598,7 +5601,7 @@
       </c>
       <c r="G123" s="5"/>
       <c r="H123" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -5622,7 +5625,7 @@
       </c>
       <c r="G124" s="5"/>
       <c r="H124" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -5646,7 +5649,7 @@
       </c>
       <c r="G125" s="5"/>
       <c r="H125" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
@@ -5670,7 +5673,7 @@
       </c>
       <c r="G126" s="5"/>
       <c r="H126" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
@@ -5694,7 +5697,7 @@
       </c>
       <c r="G127" s="5"/>
       <c r="H127" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
@@ -5718,7 +5721,7 @@
       </c>
       <c r="G128" s="5"/>
       <c r="H128" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
@@ -5742,7 +5745,7 @@
       </c>
       <c r="G129" s="5"/>
       <c r="H129" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
@@ -5766,7 +5769,7 @@
       </c>
       <c r="G130" s="5"/>
       <c r="H130" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -5800,7 +5803,7 @@
         <v>62</v>
       </c>
       <c r="H132" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -5824,7 +5827,7 @@
         <v>62</v>
       </c>
       <c r="H133" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -5848,7 +5851,7 @@
         <v>62</v>
       </c>
       <c r="H134" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
@@ -5872,7 +5875,7 @@
         <v>62</v>
       </c>
       <c r="H135" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -5896,7 +5899,7 @@
         <v>62</v>
       </c>
       <c r="H136" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -5920,7 +5923,7 @@
         <v>68</v>
       </c>
       <c r="H137" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
@@ -5944,7 +5947,7 @@
         <v>68</v>
       </c>
       <c r="H138" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
@@ -5968,7 +5971,7 @@
         <v>68</v>
       </c>
       <c r="H139" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
@@ -5992,7 +5995,7 @@
         <v>68</v>
       </c>
       <c r="H140" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -6016,7 +6019,7 @@
         <v>68</v>
       </c>
       <c r="H141" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
@@ -6040,7 +6043,7 @@
         <v>74</v>
       </c>
       <c r="H142" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -6064,7 +6067,7 @@
         <v>74</v>
       </c>
       <c r="H143" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
@@ -6088,7 +6091,7 @@
         <v>74</v>
       </c>
       <c r="H144" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
@@ -6112,7 +6115,7 @@
         <v>78</v>
       </c>
       <c r="H145" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -6136,7 +6139,7 @@
         <v>78</v>
       </c>
       <c r="H146" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -6170,7 +6173,7 @@
       </c>
       <c r="G148" s="5"/>
       <c r="H148" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -6194,7 +6197,7 @@
       </c>
       <c r="G149" s="5"/>
       <c r="H149" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
@@ -6218,7 +6221,7 @@
       </c>
       <c r="G150" s="5"/>
       <c r="H150" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -6242,7 +6245,7 @@
       </c>
       <c r="G151" s="5"/>
       <c r="H151" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -6266,7 +6269,7 @@
       </c>
       <c r="G152" s="5"/>
       <c r="H152" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -6298,7 +6301,7 @@
         <v>133</v>
       </c>
       <c r="H154" s="5" t="s">
-        <v>272</v>
+        <v>346</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
@@ -6332,7 +6335,7 @@
         <v>47</v>
       </c>
       <c r="H156" s="5" t="s">
-        <v>272</v>
+        <v>341</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
@@ -6364,7 +6367,7 @@
       <c r="F158" s="5"/>
       <c r="G158" s="5"/>
       <c r="H158" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -6386,7 +6389,7 @@
       <c r="F159" s="5"/>
       <c r="G159" s="5"/>
       <c r="H159" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -6408,7 +6411,7 @@
       <c r="F160" s="5"/>
       <c r="G160" s="5"/>
       <c r="H160" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -6442,7 +6445,7 @@
         <v>90</v>
       </c>
       <c r="H162" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
@@ -6466,7 +6469,7 @@
         <v>90</v>
       </c>
       <c r="H163" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
@@ -6490,7 +6493,7 @@
         <v>90</v>
       </c>
       <c r="H164" s="5" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -6514,7 +6517,7 @@
         <v>90</v>
       </c>
       <c r="H165" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
@@ -6538,7 +6541,7 @@
         <v>90</v>
       </c>
       <c r="H166" s="5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
@@ -6562,7 +6565,7 @@
         <v>90</v>
       </c>
       <c r="H167" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
@@ -6586,7 +6589,7 @@
         <v>90</v>
       </c>
       <c r="H168" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -6610,7 +6613,7 @@
         <v>90</v>
       </c>
       <c r="H169" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
@@ -6634,7 +6637,7 @@
         <v>90</v>
       </c>
       <c r="H170" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -6658,7 +6661,7 @@
         <v>90</v>
       </c>
       <c r="H171" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -6682,7 +6685,7 @@
         <v>90</v>
       </c>
       <c r="H172" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
@@ -6706,7 +6709,7 @@
         <v>90</v>
       </c>
       <c r="H173" s="5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -6730,7 +6733,7 @@
         <v>90</v>
       </c>
       <c r="H174" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -6754,7 +6757,7 @@
         <v>90</v>
       </c>
       <c r="H175" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -6778,7 +6781,7 @@
         <v>90</v>
       </c>
       <c r="H176" s="5" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
@@ -6810,7 +6813,7 @@
       <c r="F178" s="5"/>
       <c r="G178" s="5"/>
       <c r="H178" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
@@ -6854,7 +6857,7 @@
       </c>
       <c r="G181" s="5"/>
       <c r="H181" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -6878,7 +6881,7 @@
       </c>
       <c r="G182" s="5"/>
       <c r="H182" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -6902,7 +6905,7 @@
       </c>
       <c r="G183" s="5"/>
       <c r="H183" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
@@ -6926,7 +6929,7 @@
       </c>
       <c r="G184" s="5"/>
       <c r="H184" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
@@ -6950,7 +6953,7 @@
       </c>
       <c r="G185" s="5"/>
       <c r="H185" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -6974,7 +6977,7 @@
       </c>
       <c r="G186" s="5"/>
       <c r="H186" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -6998,7 +7001,7 @@
       </c>
       <c r="G187" s="5"/>
       <c r="H187" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
@@ -7022,7 +7025,7 @@
       </c>
       <c r="G188" s="5"/>
       <c r="H188" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
@@ -7046,7 +7049,7 @@
       </c>
       <c r="G189" s="5"/>
       <c r="H189" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
@@ -7080,7 +7083,7 @@
       </c>
       <c r="G191" s="5"/>
       <c r="H191" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
@@ -7104,7 +7107,7 @@
       </c>
       <c r="G192" s="5"/>
       <c r="H192" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
@@ -7128,7 +7131,7 @@
       </c>
       <c r="G193" s="5"/>
       <c r="H193" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
@@ -7152,7 +7155,7 @@
       </c>
       <c r="G194" s="5"/>
       <c r="H194" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
@@ -7176,7 +7179,7 @@
       </c>
       <c r="G195" s="5"/>
       <c r="H195" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
@@ -7200,7 +7203,7 @@
       </c>
       <c r="G196" s="5"/>
       <c r="H196" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
@@ -7224,7 +7227,7 @@
       </c>
       <c r="G197" s="5"/>
       <c r="H197" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
@@ -7248,7 +7251,7 @@
       </c>
       <c r="G198" s="5"/>
       <c r="H198" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
@@ -7272,7 +7275,7 @@
       </c>
       <c r="G199" s="5"/>
       <c r="H199" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
@@ -7304,7 +7307,7 @@
         <v>133</v>
       </c>
       <c r="H201" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
@@ -7338,7 +7341,7 @@
         <v>47</v>
       </c>
       <c r="H203" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
@@ -7370,7 +7373,7 @@
       <c r="F205" s="5"/>
       <c r="G205" s="5"/>
       <c r="H205" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
@@ -7392,7 +7395,7 @@
       <c r="F206" s="5"/>
       <c r="G206" s="5"/>
       <c r="H206" s="5" t="s">
-        <v>299</v>
+        <v>342</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
@@ -7414,7 +7417,7 @@
       <c r="F207" s="5"/>
       <c r="G207" s="5"/>
       <c r="H207" s="5" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
@@ -7436,7 +7439,7 @@
       <c r="F208" s="5"/>
       <c r="G208" s="5"/>
       <c r="H208" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
@@ -7468,7 +7471,7 @@
       <c r="F210" s="5"/>
       <c r="G210" s="5"/>
       <c r="H210" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
@@ -7490,7 +7493,7 @@
       <c r="F211" s="5"/>
       <c r="G211" s="5"/>
       <c r="H211" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.2">
@@ -7512,7 +7515,7 @@
       <c r="F212" s="5"/>
       <c r="G212" s="5"/>
       <c r="H212" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
@@ -7534,7 +7537,7 @@
       <c r="F213" s="5"/>
       <c r="G213" s="5"/>
       <c r="H213" s="5" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
@@ -7556,7 +7559,7 @@
       <c r="F214" s="5"/>
       <c r="G214" s="5"/>
       <c r="H214" s="5" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
@@ -7578,7 +7581,7 @@
       <c r="F215" s="5"/>
       <c r="G215" s="5"/>
       <c r="H215" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
@@ -7600,7 +7603,7 @@
       <c r="F216" s="5"/>
       <c r="G216" s="5"/>
       <c r="H216" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
@@ -7622,7 +7625,7 @@
       <c r="F217" s="5"/>
       <c r="G217" s="5"/>
       <c r="H217" s="5" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
@@ -7644,7 +7647,7 @@
       <c r="F218" s="5"/>
       <c r="G218" s="5"/>
       <c r="H218" s="5" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
@@ -7666,7 +7669,7 @@
       <c r="F219" s="5"/>
       <c r="G219" s="5"/>
       <c r="H219" s="5" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.2">
@@ -7710,7 +7713,7 @@
       </c>
       <c r="G222" s="5"/>
       <c r="H222" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.2">
@@ -7734,7 +7737,7 @@
       </c>
       <c r="G223" s="5"/>
       <c r="H223" s="5" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
@@ -7758,7 +7761,7 @@
       </c>
       <c r="G224" s="5"/>
       <c r="H224" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.2">
@@ -7782,7 +7785,7 @@
       </c>
       <c r="G225" s="5"/>
       <c r="H225" s="5" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.2">
@@ -7806,7 +7809,7 @@
       </c>
       <c r="G226" s="5"/>
       <c r="H226" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.2">
@@ -7840,7 +7843,7 @@
       </c>
       <c r="G228" s="5"/>
       <c r="H228" s="5" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.2">
@@ -7864,7 +7867,7 @@
       </c>
       <c r="G229" s="5"/>
       <c r="H229" s="5" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.2">
@@ -7888,7 +7891,7 @@
       </c>
       <c r="G230" s="5"/>
       <c r="H230" s="5" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.2">
@@ -7912,7 +7915,7 @@
       </c>
       <c r="G231" s="5"/>
       <c r="H231" s="5" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
@@ -7944,7 +7947,7 @@
         <v>133</v>
       </c>
       <c r="H233" s="5" t="s">
-        <v>317</v>
+        <v>347</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.2">
@@ -7975,7 +7978,7 @@
         <v>47</v>
       </c>
       <c r="H235" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.2">
@@ -8005,7 +8008,7 @@
       <c r="F237" s="5"/>
       <c r="G237" s="5"/>
       <c r="H237" s="5" t="s">
-        <v>319</v>
+        <v>348</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.2">
@@ -8025,7 +8028,7 @@
       <c r="F238" s="5"/>
       <c r="G238" s="5"/>
       <c r="H238" s="5" t="s">
-        <v>321</v>
+        <v>349</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.2">
@@ -8045,7 +8048,7 @@
       <c r="F239" s="5"/>
       <c r="G239" s="5"/>
       <c r="H239" s="5" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.2">
@@ -8075,7 +8078,7 @@
       <c r="F241" s="5"/>
       <c r="G241" s="5"/>
       <c r="H241" s="5" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
@@ -8105,7 +8108,7 @@
       <c r="F243" s="5"/>
       <c r="G243" s="5"/>
       <c r="H243" s="5" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="244" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -8136,7 +8139,7 @@
         <v>116</v>
       </c>
       <c r="H246" s="1" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="247" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8164,7 +8167,7 @@
         <v>119</v>
       </c>
       <c r="H248" s="1" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="249" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8187,7 +8190,7 @@
         <v>119</v>
       </c>
       <c r="H249" s="1" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="250" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8210,7 +8213,7 @@
         <v>119</v>
       </c>
       <c r="H250" s="1" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="251" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8233,7 +8236,7 @@
         <v>123</v>
       </c>
       <c r="H251" s="1" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="252" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8261,7 +8264,7 @@
         <v>47</v>
       </c>
       <c r="H253" s="1" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="254" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8286,7 +8289,7 @@
         <v>46</v>
       </c>
       <c r="H255" s="1" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="256" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8306,7 +8309,7 @@
         <v>46</v>
       </c>
       <c r="H256" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="257" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8326,7 +8329,7 @@
         <v>46</v>
       </c>
       <c r="H257" s="1" t="s">
-        <v>332</v>
+        <v>350</v>
       </c>
     </row>
     <row r="258" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8346,7 +8349,7 @@
         <v>46</v>
       </c>
       <c r="H258" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="259" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8371,7 +8374,7 @@
         <v>46</v>
       </c>
       <c r="H260" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="261" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -8400,7 +8403,7 @@
         <v>50</v>
       </c>
       <c r="H263" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="264" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8426,7 +8429,7 @@
         <v>80</v>
       </c>
       <c r="H265" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="266" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8452,7 +8455,7 @@
         <v>133</v>
       </c>
       <c r="H267" s="1" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
     </row>
     <row r="268" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8480,7 +8483,7 @@
         <v>47</v>
       </c>
       <c r="H269" s="1" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="270" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8503,7 +8506,7 @@
       </c>
       <c r="E271" s="2"/>
       <c r="H271" s="1" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="272" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8521,7 +8524,7 @@
       </c>
       <c r="E272" s="2"/>
       <c r="H272" s="1" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="273" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8539,7 +8542,7 @@
       </c>
       <c r="E273" s="2"/>
       <c r="H273" s="1" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
     </row>
     <row r="274" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8557,7 +8560,7 @@
       </c>
       <c r="E274" s="2"/>
       <c r="H274" s="1" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="275" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8580,7 +8583,7 @@
       </c>
       <c r="E276" s="2"/>
       <c r="H276" s="1" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="277" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -8609,7 +8612,7 @@
         <v>50</v>
       </c>
       <c r="H279" s="1" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="280" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8635,7 +8638,7 @@
         <v>80</v>
       </c>
       <c r="H281" s="1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="282" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8661,7 +8664,7 @@
         <v>133</v>
       </c>
       <c r="H283" s="1" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row r="284" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8687,7 +8690,7 @@
         <v>47</v>
       </c>
       <c r="H285" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="286" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8710,7 +8713,7 @@
       </c>
       <c r="E287" s="2"/>
       <c r="H287" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="288" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8728,7 +8731,7 @@
       </c>
       <c r="E288" s="2"/>
       <c r="H288" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="289" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8746,7 +8749,7 @@
       </c>
       <c r="E289" s="2"/>
       <c r="H289" s="1" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
     </row>
     <row r="290" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8764,7 +8767,7 @@
       </c>
       <c r="E290" s="2"/>
       <c r="H290" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
     </row>
     <row r="291" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8787,7 +8790,7 @@
       </c>
       <c r="E292" s="2"/>
       <c r="H292" s="1" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>